<commit_message>
chore(dod): actualiza observaciones con rutas de archivos
</commit_message>
<xml_diff>
--- a/docs/dod/PRY3211_Exp2_S5_formato_de_respuesta_Definition_Of_Done_Vistas_de_Diseño.xlsx
+++ b/docs/dod/PRY3211_Exp2_S5_formato_de_respuesta_Definition_Of_Done_Vistas_de_Diseño.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/Downloads/ISW_S5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/Desktop/semana5-vistas/docs/dod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCFC7F5-939B-F148-A90F-50268F7F1A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124822D8-478C-5348-93C7-452C25A0087C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-720" windowWidth="36820" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>DEFINICION DEL  DOD</t>
   </si>
@@ -236,12 +236,15 @@
   <si>
     <t>Mockups Administrador</t>
   </si>
+  <si>
+    <t>Nota:Evidencias en carpeta docs/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,49 +256,58 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="50"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -303,6 +315,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -510,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,6 +570,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -559,12 +587,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,9 +598,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1202,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1234,10 +1254,10 @@
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1247,12 +1267,12 @@
         <v>3</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
       <c r="L2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1267,8 +1287,8 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1276,11 +1296,11 @@
         <v>3</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="7">
         <f>SUM(D2:D5)/12</f>
         <v>0.83333333333333337</v>
@@ -1299,8 +1319,8 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1308,11 +1328,11 @@
         <v>2</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
       <c r="I4" s="7">
         <f>SUM(D6:D9)/12</f>
         <v>0.75</v>
@@ -1331,8 +1351,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1340,19 +1360,19 @@
         <v>2</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
       <c r="I5" s="7">
         <f>SUM(D10,D13)/6</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
-      <c r="B6" s="27" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1362,19 +1382,19 @@
         <v>3</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="7">
         <f>SUM(D14,D17)/6</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1382,19 +1402,19 @@
         <v>2</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="7">
         <f>SUM(MediaArtefacto1:MediaArtefacto3)/3</f>
         <v>0.80555555555555569</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
@@ -1406,8 +1426,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1417,8 +1437,8 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1432,8 +1452,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1445,8 +1465,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1458,8 +1478,8 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:15" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="3" t="s">
         <v>16</v>
       </c>
@@ -1473,8 +1493,8 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="27" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1490,8 +1510,8 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1505,8 +1525,8 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1520,8 +1540,8 @@
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1535,10 +1555,10 @@
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1554,8 +1574,8 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="3" t="s">
         <v>9</v>
       </c>
@@ -1569,8 +1589,8 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1581,8 +1601,8 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="3" t="s">
         <v>16</v>
       </c>
@@ -1591,8 +1611,8 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
-      <c r="B22" s="27" t="s">
+      <c r="A22" s="18"/>
+      <c r="B22" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1603,8 +1623,8 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="18"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="3" t="s">
         <v>9</v>
       </c>
@@ -1613,8 +1633,8 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
-      <c r="B24" s="18"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="3" t="s">
         <v>14</v>
       </c>
@@ -1623,8 +1643,8 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="3" t="s">
         <v>16</v>
       </c>
@@ -1633,28 +1653,31 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
+      <c r="A26" s="18"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
+      <c r="A27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
+      <c r="A28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
+      <c r="A29" s="18"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
+      <c r="A30" s="18"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
+      <c r="A31" s="18"/>
+      <c r="C31" s="28" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
+      <c r="A32" s="18"/>
     </row>
     <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="21"/>
+      <c r="A33" s="18"/>
     </row>
     <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2668,41 +2691,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="25">
+      <c r="B2" s="26">
         <f>Checklist!I7</f>
         <v>0.80555555555555569</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="24"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="25"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="24"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3696,27 +3719,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d0daa353-f819-43d1-badf-ce69fea8800d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Fecha_x0020_de_x0020_creaci_x00f3_n xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
-    <TaxCatchAll xmlns="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d" xsi:nil="true"/>
-    <Fechayhora xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
-    <SharedWithUsers xmlns="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010070BFDEA41A5D8B46AA5DA2E2389CBE4E" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="672700c7c1e39a78a362f54b21ce1efa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d0daa353-f819-43d1-badf-ce69fea8800d" xmlns:ns3="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3db37e5c6f54565a9911855e2c96e577" ns2:_="" ns3:_="">
     <xsd:import namespace="d0daa353-f819-43d1-badf-ce69fea8800d"/>
@@ -3971,6 +3973,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d0daa353-f819-43d1-badf-ce69fea8800d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Fecha_x0020_de_x0020_creaci_x00f3_n xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
+    <TaxCatchAll xmlns="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d" xsi:nil="true"/>
+    <Fechayhora xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
+    <SharedWithUsers xmlns="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="d0daa353-f819-43d1-badf-ce69fea8800d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3981,17 +4004,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A26DB7C-878E-46E5-89F2-71019BF99099}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d0daa353-f819-43d1-badf-ce69fea8800d"/>
-    <ds:schemaRef ds:uri="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81288DC1-A1A5-4A8F-86BC-34BD167F9197}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4010,6 +4022,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A26DB7C-878E-46E5-89F2-71019BF99099}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d0daa353-f819-43d1-badf-ce69fea8800d"/>
+    <ds:schemaRef ds:uri="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47A3290B-B6C1-4BEF-B4D8-BE863B785917}">
   <ds:schemaRefs>

</xml_diff>